<commit_message>
purchase report editing,generating,copying solved
</commit_message>
<xml_diff>
--- a/media/2025/Sep/2025-09-09/2025-09-09_PurchaseReport.xlsx
+++ b/media/2025/Sep/2025-09-09/2025-09-09_PurchaseReport.xlsx
@@ -724,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -979,474 +979,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" s="16">
-      <c r="A7" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Sealing ring, vehicle RG-SEAL-DIN7603-HONDA-ALU-14X22X2</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>46411422</v>
-      </c>
-      <c r="F7" t="n">
-        <v>48.16</v>
-      </c>
-      <c r="G7" t="n">
-        <v>25</v>
-      </c>
-      <c r="H7" t="n">
-        <v>25</v>
-      </c>
-      <c r="I7" t="n">
-        <v>12.04</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="N7" t="n">
-        <v>5.02</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" s="16">
-      <c r="A8" t="n">
-        <v>4</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Copper sealing ring RG-SEAL-DIN7603-CU-C-ASBESTFREE-20X26</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
-        <v>46202026</v>
-      </c>
-      <c r="F8" t="n">
-        <v>324.82</v>
-      </c>
-      <c r="G8" t="n">
-        <v>20</v>
-      </c>
-      <c r="H8" t="n">
-        <v>20</v>
-      </c>
-      <c r="I8" t="n">
-        <v>64.95999999999999</v>
-      </c>
-      <c r="J8" t="n">
-        <v>3.25</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L8" t="n">
-        <v>30.87</v>
-      </c>
-      <c r="M8" t="n">
-        <v>3.09</v>
-      </c>
-      <c r="N8" t="n">
-        <v>33.96</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1" s="16">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Radiator anti-freeze RADANTIFREZ-OAT-RED-20LTR</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
-        <v>892352020</v>
-      </c>
-      <c r="F9" t="n">
-        <v>108</v>
-      </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" t="n">
-        <v>108.01</v>
-      </c>
-      <c r="J9" t="n">
-        <v>108.01</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L9" t="n">
-        <v>1026.1</v>
-      </c>
-      <c r="M9" t="n">
-        <v>102.61</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1128.71</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="16">
-      <c r="A10" t="n">
-        <v>6</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Halogen bulb, vehicle BULB-(H9005-HB3)-P20D-12V-60W</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>7201103</v>
-      </c>
-      <c r="F10" t="n">
-        <v>15.45</v>
-      </c>
-      <c r="G10" t="n">
-        <v>5</v>
-      </c>
-      <c r="H10" t="n">
-        <v>5</v>
-      </c>
-      <c r="I10" t="n">
-        <v>77.25</v>
-      </c>
-      <c r="J10" t="n">
-        <v>15.45</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L10" t="n">
-        <v>146.77</v>
-      </c>
-      <c r="M10" t="n">
-        <v>14.68</v>
-      </c>
-      <c r="N10" t="n">
-        <v>161.45</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1" s="16">
-      <c r="A11" t="n">
-        <v>7</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Indicator/brake light bulb, vehicle BULB-INDCTR/BRK-P21/5W-BAY15D-12V-21/5W</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>7201341</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2.87</v>
-      </c>
-      <c r="G11" t="n">
-        <v>20</v>
-      </c>
-      <c r="H11" t="n">
-        <v>20</v>
-      </c>
-      <c r="I11" t="n">
-        <v>57.4</v>
-      </c>
-      <c r="J11" t="n">
-        <v>2.87</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L11" t="n">
-        <v>27.26</v>
-      </c>
-      <c r="M11" t="n">
-        <v>2.73</v>
-      </c>
-      <c r="N11" t="n">
-        <v>29.99</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" s="16">
-      <c r="A12" t="n">
-        <v>8</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Silicone spray, universal CURTAIN-TRACK-LUBE-300G</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>893125080</v>
-      </c>
-      <c r="F12" t="n">
-        <v>12.95</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="n">
-        <v>12.95</v>
-      </c>
-      <c r="J12" t="n">
-        <v>12.95</v>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L12" t="n">
-        <v>123.02</v>
-      </c>
-      <c r="M12" t="n">
-        <v>12.3</v>
-      </c>
-      <c r="N12" t="n">
-        <v>135.32</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" s="16">
-      <c r="A13" t="n">
-        <v>9</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Carburettor and throttle valve cleaner THRTLVLVECLNR-400G</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>1893100</v>
-      </c>
-      <c r="F13" t="n">
-        <v>11.21</v>
-      </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="n">
-        <v>11.21</v>
-      </c>
-      <c r="J13" t="n">
-        <v>11.21</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L13" t="n">
-        <v>106.5</v>
-      </c>
-      <c r="M13" t="n">
-        <v>10.65</v>
-      </c>
-      <c r="N13" t="n">
-        <v>117.15</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="16">
-      <c r="A14" t="n">
-        <v>10</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Deodoriser DEODOR-500ML</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>89313920</v>
-      </c>
-      <c r="F14" t="n">
-        <v>34.16</v>
-      </c>
-      <c r="G14" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" t="n">
-        <v>68.31999999999999</v>
-      </c>
-      <c r="J14" t="n">
-        <v>34.16</v>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L14" t="n">
-        <v>324.52</v>
-      </c>
-      <c r="M14" t="n">
-        <v>32.45</v>
-      </c>
-      <c r="N14" t="n">
-        <v>356.97</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" s="16">
-      <c r="A15" t="n">
-        <v>11</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>wurth</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>25-06-06</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Handling FREIGHT LUMP SUM</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>996000110</v>
-      </c>
-      <c r="F15" t="n">
-        <v>14.95</v>
-      </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" t="n">
-        <v>14.95</v>
-      </c>
-      <c r="J15" t="n">
-        <v>14.95</v>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>850 %</t>
-        </is>
-      </c>
-      <c r="L15" t="n">
-        <v>142.02</v>
-      </c>
-      <c r="M15" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="N15" t="n">
-        <v>156.22</v>
-      </c>
-    </row>
+    <row r="7" ht="15.75" customHeight="1" s="16"/>
+    <row r="8" ht="15.75" customHeight="1" s="16"/>
+    <row r="9" ht="15.75" customHeight="1" s="16"/>
+    <row r="10" ht="15.75" customHeight="1" s="16"/>
+    <row r="11" ht="15.75" customHeight="1" s="16"/>
+    <row r="12" ht="15.75" customHeight="1" s="16"/>
+    <row r="13" ht="15.75" customHeight="1" s="16"/>
+    <row r="14" ht="15.75" customHeight="1" s="16"/>
+    <row r="15" ht="15.75" customHeight="1" s="16"/>
     <row r="16" ht="15.75" customHeight="1" s="16"/>
     <row r="17" ht="15.75" customHeight="1" s="16"/>
     <row r="18" ht="15.75" customHeight="1" s="16"/>

</xml_diff>

<commit_message>
completed PurchaseReport generating module
</commit_message>
<xml_diff>
--- a/media/2025/Sep/2025-09-09/2025-09-09_PurchaseReport.xlsx
+++ b/media/2025/Sep/2025-09-09/2025-09-09_PurchaseReport.xlsx
@@ -724,7 +724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -895,20 +895,30 @@
           <t>TYRMALCN00009</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>130</v>
-      </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>130</v>
-      </c>
-      <c r="J5" t="n">
-        <v>65</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>130.00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>130.00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>65.00</t>
+        </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -949,20 +959,30 @@
           <t>SG-FRT0000001</t>
         </is>
       </c>
-      <c r="F6" t="n">
-        <v>40</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>40</v>
-      </c>
-      <c r="J6" t="n">
-        <v>40</v>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -979,15 +999,564 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" s="16"/>
-    <row r="8" ht="15.75" customHeight="1" s="16"/>
-    <row r="9" ht="15.75" customHeight="1" s="16"/>
-    <row r="10" ht="15.75" customHeight="1" s="16"/>
-    <row r="11" ht="15.75" customHeight="1" s="16"/>
-    <row r="12" ht="15.75" customHeight="1" s="16"/>
-    <row r="13" ht="15.75" customHeight="1" s="16"/>
-    <row r="14" ht="15.75" customHeight="1" s="16"/>
-    <row r="15" ht="15.75" customHeight="1" s="16"/>
+    <row r="7" ht="15.75" customHeight="1" s="16">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Sealing ring, vehicle RG-SEAL-DIN7603-HONDA-ALU-14X22X2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>046411422</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>48.16</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>12.04</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L7" t="n">
+        <v>4.56</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="N7" t="n">
+        <v>5.02</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" s="16">
+      <c r="A8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Copper sealing ring RG-SEAL-DIN7603-CU-C-ASBESTFREE-20X26</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>046202026</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>324.82</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>64.96</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>30.87</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3.09</v>
+      </c>
+      <c r="N8" t="n">
+        <v>33.96</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="16">
+      <c r="A9" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Radiator anti-freeze RADANTIFREZ-OAT-RED-20LTR</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0892352020</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>108.00</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>108.01</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>108.01</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>1026.1</v>
+      </c>
+      <c r="M9" t="n">
+        <v>102.61</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1128.71</v>
+      </c>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="16">
+      <c r="A10" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Halogen bulb, vehicle BULB-(H9005-HB3)-P20D-12V-60W</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>07201103</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>15.45</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>77.25</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>146.77</v>
+      </c>
+      <c r="M10" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="N10" t="n">
+        <v>161.45</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" s="16">
+      <c r="A11" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Indicator/brake light bulb, vehicle BULB-INDCTR/BRK-P21/5W-BAY15D-12V-21/5W</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>07201341</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2.87</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>57.40</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>27.26</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="N11" t="n">
+        <v>29.99</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="16">
+      <c r="A12" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Silicone spray, universal CURTAIN-TRACK-LUBE-300G</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0893125080</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12.95</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>12.95</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>12.95</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>123.02</v>
+      </c>
+      <c r="M12" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="N12" t="n">
+        <v>135.32</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="16">
+      <c r="A13" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Carburettor and throttle valve cleaner THRTLVLVECLNR-400G</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>1893100</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>11.21</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>11.21</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>106.5</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="N13" t="n">
+        <v>117.15</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="16">
+      <c r="A14" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Deodoriser DEODOR-500ML</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>089313920</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>34.16</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>68.32</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>34.16</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>324.52</v>
+      </c>
+      <c r="M14" t="n">
+        <v>32.45</v>
+      </c>
+      <c r="N14" t="n">
+        <v>356.97</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="16">
+      <c r="A15" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>wurth</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>25-06-06</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Handling FREIGHT LUMP SUM</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0996000110</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>14.95</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>14.95</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>14.95</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>850 %</t>
+        </is>
+      </c>
+      <c r="L15" t="n">
+        <v>142.02</v>
+      </c>
+      <c r="M15" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="N15" t="n">
+        <v>156.22</v>
+      </c>
+    </row>
     <row r="16" ht="15.75" customHeight="1" s="16"/>
     <row r="17" ht="15.75" customHeight="1" s="16"/>
     <row r="18" ht="15.75" customHeight="1" s="16"/>

</xml_diff>